<commit_message>
brand page 연동, 수정
</commit_message>
<xml_diff>
--- a/KFQ_Django/#Document/2차_DB_만들기.xlsx
+++ b/KFQ_Django/#Document/2차_DB_만들기.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\19tak\ai 개발자 과정\prj2\work\KFQ_Django\#Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5292C595-0106-48EC-BAEE-6936009A0D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50632E8A-D438-41D4-99AC-50D823D2ABDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRM_classlist" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="326">
   <si>
     <t>Y</t>
   </si>
@@ -782,10 +782,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전기정보통신 공학부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기계공학과</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -827,6 +823,250 @@
   </si>
   <si>
     <t>응용수학과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ai1@kfq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ai2@kfq.com</t>
+  </si>
+  <si>
+    <t>ai3@kfq.com</t>
+  </si>
+  <si>
+    <t>ai4@kfq.com</t>
+  </si>
+  <si>
+    <t>ai5@kfq.com</t>
+  </si>
+  <si>
+    <t>ai6@kfq.com</t>
+  </si>
+  <si>
+    <t>ai7@kfq.com</t>
+  </si>
+  <si>
+    <t>ai8@kfq.com</t>
+  </si>
+  <si>
+    <t>ai9@kfq.com</t>
+  </si>
+  <si>
+    <t>ai10@kfq.com</t>
+  </si>
+  <si>
+    <t>ai11@kfq.com</t>
+  </si>
+  <si>
+    <t>ai12@kfq.com</t>
+  </si>
+  <si>
+    <t>ai13@kfq.com</t>
+  </si>
+  <si>
+    <t>ai14@kfq.com</t>
+  </si>
+  <si>
+    <t>ai15@kfq.com</t>
+  </si>
+  <si>
+    <t>ai16@kfq.com</t>
+  </si>
+  <si>
+    <t>ai17@kfq.com</t>
+  </si>
+  <si>
+    <t>ai18@kfq.com</t>
+  </si>
+  <si>
+    <t>ai19@kfq.com</t>
+  </si>
+  <si>
+    <t>ai20@kfq.com</t>
+  </si>
+  <si>
+    <t>ai21@kfq.com</t>
+  </si>
+  <si>
+    <t>ai22@kfq.com</t>
+  </si>
+  <si>
+    <t>ai23@kfq.com</t>
+  </si>
+  <si>
+    <t>ai24@kfq.com</t>
+  </si>
+  <si>
+    <t>ai25@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata1@kfq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bigdata2@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata3@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata4@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata5@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata6@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata7@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata8@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata9@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata10@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata11@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata12@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata13@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata14@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata15@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata16@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata17@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata18@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata19@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata20@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata21@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata22@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata23@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata24@kfq.com</t>
+  </si>
+  <si>
+    <t>bigdata25@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory1@kfq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>smartfactory2@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory3@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory4@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory5@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory6@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory7@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory8@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory9@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory10@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory11@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory12@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory13@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory14@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory15@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory16@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory17@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory18@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory19@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory20@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory21@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory22@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory23@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory24@kfq.com</t>
+  </si>
+  <si>
+    <t>smartfactory25@kfq.com</t>
+  </si>
+  <si>
+    <t>배고픈대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐먹을과</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -834,7 +1074,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,6 +1118,15 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -917,12 +1166,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -947,9 +1199,13 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6279,15 +6535,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D1E8E30-2B9A-4360-B71C-24AEAC880BC7}">
-  <dimension ref="E1:M80"/>
+  <dimension ref="C1:M77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="5:13">
+    <row r="1" spans="3:13">
+      <c r="C1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" t="s">
+        <v>247</v>
+      </c>
       <c r="E1" t="s">
         <v>194</v>
       </c>
@@ -6316,18 +6578,36 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="5:13">
+    <row r="3" spans="3:13">
+      <c r="C3" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3">
+        <v>1111</v>
+      </c>
       <c r="E3" t="s">
         <v>203</v>
       </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
       <c r="M3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="5:13">
+    <row r="4" spans="3:13">
+      <c r="C4" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4">
+        <v>1111</v>
+      </c>
       <c r="E4" t="s">
         <v>204</v>
       </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
       <c r="H4" t="s">
         <v>226</v>
       </c>
@@ -6335,10 +6615,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="5:13">
+    <row r="5" spans="3:13">
+      <c r="C5" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5">
+        <v>1111</v>
+      </c>
       <c r="E5" t="s">
         <v>205</v>
       </c>
+      <c r="F5">
+        <v>25</v>
+      </c>
       <c r="H5" t="s">
         <v>227</v>
       </c>
@@ -6346,10 +6635,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="5:13">
+    <row r="6" spans="3:13">
+      <c r="C6" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6">
+        <v>1111</v>
+      </c>
       <c r="E6" t="s">
         <v>206</v>
       </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
       <c r="H6" t="s">
         <v>228</v>
       </c>
@@ -6357,10 +6655,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="5:13">
+    <row r="7" spans="3:13">
+      <c r="C7" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D7">
+        <v>1111</v>
+      </c>
       <c r="E7" t="s">
         <v>207</v>
       </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
       <c r="H7" t="s">
         <v>229</v>
       </c>
@@ -6368,10 +6675,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="5:13">
+    <row r="8" spans="3:13">
+      <c r="C8" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8">
+        <v>1111</v>
+      </c>
       <c r="E8" t="s">
         <v>208</v>
       </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
       <c r="H8" t="s">
         <v>230</v>
       </c>
@@ -6379,10 +6695,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="5:13">
+    <row r="9" spans="3:13">
+      <c r="C9" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="D9">
+        <v>1111</v>
+      </c>
       <c r="E9" t="s">
         <v>209</v>
       </c>
+      <c r="F9">
+        <v>25</v>
+      </c>
       <c r="H9" t="s">
         <v>231</v>
       </c>
@@ -6390,10 +6715,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="5:13">
+    <row r="10" spans="3:13">
+      <c r="C10" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D10">
+        <v>1111</v>
+      </c>
       <c r="E10" t="s">
         <v>210</v>
       </c>
+      <c r="F10">
+        <v>27</v>
+      </c>
       <c r="H10" t="s">
         <v>232</v>
       </c>
@@ -6401,10 +6735,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="5:13">
+    <row r="11" spans="3:13">
+      <c r="C11" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11">
+        <v>1111</v>
+      </c>
       <c r="E11" t="s">
         <v>211</v>
       </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
       <c r="H11" t="s">
         <v>233</v>
       </c>
@@ -6412,10 +6755,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="5:13">
+    <row r="12" spans="3:13">
+      <c r="C12" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12">
+        <v>1111</v>
+      </c>
       <c r="E12" t="s">
         <v>212</v>
       </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
       <c r="H12" t="s">
         <v>234</v>
       </c>
@@ -6423,10 +6775,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="5:13">
+    <row r="13" spans="3:13">
+      <c r="C13" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13">
+        <v>1111</v>
+      </c>
       <c r="E13" t="s">
         <v>208</v>
       </c>
+      <c r="F13">
+        <v>25</v>
+      </c>
       <c r="H13" t="s">
         <v>235</v>
       </c>
@@ -6434,98 +6795,182 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="5:13">
+    <row r="14" spans="3:13">
+      <c r="C14" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14">
+        <v>1111</v>
+      </c>
       <c r="E14" t="s">
         <v>213</v>
       </c>
+      <c r="F14">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>324</v>
+      </c>
       <c r="H14" t="s">
-        <v>236</v>
+        <v>325</v>
       </c>
       <c r="M14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="5:13">
+    <row r="15" spans="3:13">
+      <c r="C15" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D15">
+        <v>1111</v>
+      </c>
       <c r="E15" t="s">
         <v>214</v>
       </c>
+      <c r="F15">
+        <v>28</v>
+      </c>
       <c r="H15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="5:13">
+    <row r="16" spans="3:13">
+      <c r="C16" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16">
+        <v>1111</v>
+      </c>
       <c r="E16" t="s">
         <v>192</v>
       </c>
+      <c r="F16">
+        <v>25</v>
+      </c>
       <c r="H16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M16">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="5:13">
+    <row r="17" spans="3:13">
+      <c r="C17" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D17">
+        <v>1111</v>
+      </c>
       <c r="E17" t="s">
         <v>215</v>
       </c>
+      <c r="F17">
+        <v>25</v>
+      </c>
       <c r="H17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="5:13">
+    <row r="18" spans="3:13">
+      <c r="C18" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D18">
+        <v>1111</v>
+      </c>
       <c r="E18" t="s">
         <v>216</v>
       </c>
+      <c r="F18">
+        <v>25</v>
+      </c>
       <c r="H18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="5:13">
+    <row r="19" spans="3:13">
+      <c r="C19" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D19">
+        <v>1111</v>
+      </c>
       <c r="E19" t="s">
         <v>217</v>
       </c>
+      <c r="F19">
+        <v>25</v>
+      </c>
       <c r="H19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M19">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="5:13">
+    <row r="20" spans="3:13">
+      <c r="C20" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D20">
+        <v>1111</v>
+      </c>
       <c r="E20" t="s">
         <v>218</v>
       </c>
+      <c r="F20">
+        <v>25</v>
+      </c>
       <c r="H20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M20">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="5:13">
+    <row r="21" spans="3:13">
+      <c r="C21" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21">
+        <v>1111</v>
+      </c>
       <c r="E21" t="s">
         <v>219</v>
       </c>
+      <c r="F21">
+        <v>25</v>
+      </c>
       <c r="H21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M21">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="5:13">
+    <row r="22" spans="3:13">
+      <c r="C22" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22">
+        <v>1111</v>
+      </c>
       <c r="E22" t="s">
         <v>220</v>
       </c>
+      <c r="F22">
+        <v>25</v>
+      </c>
       <c r="H22" t="s">
         <v>233</v>
       </c>
@@ -6533,467 +6978,967 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="5:13">
+    <row r="23" spans="3:13">
+      <c r="C23" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D23">
+        <v>1111</v>
+      </c>
       <c r="E23" t="s">
         <v>221</v>
       </c>
+      <c r="F23">
+        <v>25</v>
+      </c>
       <c r="H23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M23">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="5:13">
+    <row r="24" spans="3:13">
+      <c r="C24" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D24">
+        <v>1111</v>
+      </c>
       <c r="E24" t="s">
         <v>222</v>
       </c>
+      <c r="F24">
+        <v>25</v>
+      </c>
       <c r="H24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M24">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="5:13">
+    <row r="25" spans="3:13">
+      <c r="C25" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D25">
+        <v>1111</v>
+      </c>
       <c r="E25" t="s">
         <v>223</v>
       </c>
+      <c r="F25">
+        <v>25</v>
+      </c>
       <c r="H25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M25">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="5:13">
+    <row r="26" spans="3:13">
+      <c r="C26" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D26">
+        <v>1111</v>
+      </c>
       <c r="E26" t="s">
         <v>221</v>
       </c>
+      <c r="F26">
+        <v>25</v>
+      </c>
       <c r="H26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M26">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="5:13">
+    <row r="27" spans="3:13">
+      <c r="C27" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D27">
+        <v>1111</v>
+      </c>
       <c r="E27" t="s">
         <v>224</v>
       </c>
+      <c r="F27">
+        <v>25</v>
+      </c>
       <c r="H27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M27">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="5:13">
+    <row r="28" spans="3:13">
+      <c r="C28" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D28">
+        <v>1111</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28">
+        <v>25</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13">
+      <c r="C29" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D29">
+        <v>1111</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F29">
+        <v>25</v>
+      </c>
+      <c r="M29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13">
+      <c r="C30" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D30">
+        <v>1111</v>
+      </c>
       <c r="E30" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F30">
+        <v>25</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13">
+      <c r="C31" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D31">
+        <v>1111</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F31">
+        <v>25</v>
+      </c>
+      <c r="M31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13">
+      <c r="C32" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D32">
+        <v>1111</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32">
+        <v>25</v>
+      </c>
+      <c r="M32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13">
+      <c r="C33" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D33">
+        <v>1111</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33">
+        <v>25</v>
+      </c>
+      <c r="M33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13">
+      <c r="C34" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D34">
+        <v>1111</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F34">
+        <v>25</v>
+      </c>
+      <c r="M34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13">
+      <c r="C35" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D35">
+        <v>1111</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35">
+        <v>25</v>
+      </c>
+      <c r="M35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13">
+      <c r="C36" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D36">
+        <v>1111</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F36">
+        <v>25</v>
+      </c>
+      <c r="M36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13">
+      <c r="C37" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D37">
+        <v>1111</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37">
+        <v>25</v>
+      </c>
+      <c r="M37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13">
+      <c r="C38" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D38">
+        <v>1111</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38">
+        <v>25</v>
+      </c>
+      <c r="M38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13">
+      <c r="C39" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D39">
+        <v>1111</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F39">
+        <v>25</v>
+      </c>
+      <c r="M39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13">
+      <c r="C40" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D40">
+        <v>1111</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="M30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="5:13">
-      <c r="E31" s="5" t="s">
+      <c r="F40">
+        <v>25</v>
+      </c>
+      <c r="M40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="3:13">
+      <c r="C41" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D41">
+        <v>1111</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="M31">
+      <c r="F41">
+        <v>25</v>
+      </c>
+      <c r="M41">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13">
+      <c r="C42" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D42">
+        <v>1111</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F42">
+        <v>25</v>
+      </c>
+      <c r="M42">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="3:13">
+      <c r="C43" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D43">
+        <v>1111</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F43">
+        <v>25</v>
+      </c>
+      <c r="M43">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13">
+      <c r="C44" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D44">
+        <v>1111</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F44">
+        <v>25</v>
+      </c>
+      <c r="M44">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13">
+      <c r="C45" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="D45">
+        <v>1111</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F45">
+        <v>25</v>
+      </c>
+      <c r="M45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="3:13">
+      <c r="C46" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D46">
+        <v>1111</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F46">
+        <v>25</v>
+      </c>
+      <c r="M46">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="3:13">
+      <c r="C47" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="D47">
+        <v>1111</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F47">
+        <v>25</v>
+      </c>
+      <c r="M47">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="3:13">
+      <c r="C48" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="D48">
+        <v>1111</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F48">
+        <v>25</v>
+      </c>
+      <c r="M48">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="3:13">
+      <c r="C49" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D49">
+        <v>1111</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49">
+        <v>25</v>
+      </c>
+      <c r="M49">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="3:13">
+      <c r="C50" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D50">
+        <v>1111</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F50">
+        <v>25</v>
+      </c>
+      <c r="M50">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="3:13">
+      <c r="C51" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="D51">
+        <v>1111</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F51">
+        <v>25</v>
+      </c>
+      <c r="M51">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="3:13">
+      <c r="C52" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="D52">
+        <v>1111</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F52">
+        <v>25</v>
+      </c>
+      <c r="M52">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="3:13">
+      <c r="C53" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D53">
+        <v>1111</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F53">
+        <v>25</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="3:13">
+      <c r="C54" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D54">
+        <v>1111</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F54">
+        <v>25</v>
+      </c>
+      <c r="M54">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="5:13">
-      <c r="E32" s="5" t="s">
+    <row r="55" spans="3:13">
+      <c r="C55" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="D55">
+        <v>1111</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="M32">
+      <c r="F55">
+        <v>25</v>
+      </c>
+      <c r="M55">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="5:13">
-      <c r="E33" s="5" t="s">
+    <row r="56" spans="3:13">
+      <c r="C56" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D56">
+        <v>1111</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="M33">
+      <c r="F56">
+        <v>25</v>
+      </c>
+      <c r="M56">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="5:13">
-      <c r="E34" s="5" t="s">
+    <row r="57" spans="3:13">
+      <c r="C57" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D57">
+        <v>1111</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="M34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="5:13">
-      <c r="E35" s="5" t="s">
+      <c r="F57">
+        <v>25</v>
+      </c>
+      <c r="M57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="3:13">
+      <c r="C58" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D58">
+        <v>1111</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="M35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="5:13">
-      <c r="E36" s="5" t="s">
+      <c r="F58">
+        <v>25</v>
+      </c>
+      <c r="M58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="3:13">
+      <c r="C59" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D59">
+        <v>1111</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="M36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="5:13">
-      <c r="E37" s="5" t="s">
+      <c r="F59">
+        <v>25</v>
+      </c>
+      <c r="M59">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="3:13">
+      <c r="C60" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="D60">
+        <v>1111</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="M37">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="5:13">
-      <c r="E38" s="5" t="s">
+      <c r="F60">
+        <v>25</v>
+      </c>
+      <c r="M60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="3:13">
+      <c r="C61" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D61">
+        <v>1111</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="M38">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="5:13">
-      <c r="E39" s="5" t="s">
+      <c r="F61">
+        <v>25</v>
+      </c>
+      <c r="M61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="3:13">
+      <c r="C62" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D62">
+        <v>1111</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="M39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="5:13">
-      <c r="E40" s="5" t="s">
+      <c r="F62">
+        <v>25</v>
+      </c>
+      <c r="M62">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="3:13">
+      <c r="C63" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="D63">
+        <v>1111</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="M40">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="5:13">
-      <c r="E41" s="5" t="s">
+      <c r="F63">
+        <v>25</v>
+      </c>
+      <c r="M63">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="3:13">
+      <c r="C64" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="D64">
+        <v>1111</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="M41">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="5:13">
-      <c r="E42" s="5" t="s">
+      <c r="F64">
+        <v>25</v>
+      </c>
+      <c r="M64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="3:13">
+      <c r="C65" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="D65">
+        <v>1111</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="M42">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="5:13">
-      <c r="E43" s="5" t="s">
+      <c r="F65">
+        <v>25</v>
+      </c>
+      <c r="M65">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="3:13">
+      <c r="C66" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D66">
+        <v>1111</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="M43">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="5:13">
-      <c r="E44" s="5" t="s">
+      <c r="F66">
+        <v>25</v>
+      </c>
+      <c r="M66">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="3:13">
+      <c r="C67" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="D67">
+        <v>1111</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="M44">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="5:13">
-      <c r="E45" s="5" t="s">
+      <c r="F67">
+        <v>25</v>
+      </c>
+      <c r="M67">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="3:13">
+      <c r="C68" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="D68">
+        <v>1111</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="M45">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="5:13">
-      <c r="E46" s="5" t="s">
+      <c r="F68">
+        <v>25</v>
+      </c>
+      <c r="M68">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="3:13">
+      <c r="C69" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="D69">
+        <v>1111</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="M46">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="5:13">
-      <c r="E47" s="5" t="s">
+      <c r="F69">
+        <v>25</v>
+      </c>
+      <c r="M69">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="3:13">
+      <c r="C70" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D70">
+        <v>1111</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="M47">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="5:13">
-      <c r="E48" s="5" t="s">
+      <c r="F70">
+        <v>25</v>
+      </c>
+      <c r="M70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="3:13">
+      <c r="C71" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="D71">
+        <v>1111</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="M48">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="5:13">
-      <c r="E49" s="5" t="s">
+      <c r="F71">
+        <v>25</v>
+      </c>
+      <c r="M71">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="3:13">
+      <c r="C72" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="D72">
+        <v>1111</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="M49">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="5:13">
-      <c r="E50" s="5" t="s">
+      <c r="F72">
+        <v>25</v>
+      </c>
+      <c r="M72">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="3:13">
+      <c r="C73" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="D73">
+        <v>1111</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="M50">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="5:13">
-      <c r="E51" s="5" t="s">
+      <c r="F73">
+        <v>25</v>
+      </c>
+      <c r="M73">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="3:13">
+      <c r="C74" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="D74">
+        <v>1111</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="M51">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="5:13">
-      <c r="E52" s="5" t="s">
+      <c r="F74">
+        <v>25</v>
+      </c>
+      <c r="M74">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="3:13">
+      <c r="C75" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="D75">
+        <v>1111</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="M52">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="5:13">
-      <c r="E53" s="5" t="s">
+      <c r="F75">
+        <v>25</v>
+      </c>
+      <c r="M75">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="76" spans="3:13">
+      <c r="C76" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D76">
+        <v>1111</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="M53">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="5:13">
-      <c r="E54" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="M54">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="5:13">
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="5:13">
-      <c r="E56" s="5" t="s">
+      <c r="F76">
+        <v>25</v>
+      </c>
+      <c r="M76">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="3:13">
+      <c r="C77" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="D77">
+        <v>1111</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="M56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="5:13">
-      <c r="E57" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="M57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="5:13">
-      <c r="E58" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="M58">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="5:13">
-      <c r="E59" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="M59">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="5:13">
-      <c r="E60" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="M60">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="5:13">
-      <c r="E61" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="M61">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="5:13">
-      <c r="E62" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="M62">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="5:13">
-      <c r="E63" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="M63">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="5:13">
-      <c r="E64" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="M64">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="5:13">
-      <c r="E65" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="M65">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="5:13">
-      <c r="E66" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="M66">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="5:13">
-      <c r="E67" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="M67">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="5:13">
-      <c r="E68" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="M68">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="69" spans="5:13">
-      <c r="E69" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="M69">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70" spans="5:13">
-      <c r="E70" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="M70">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="5:13">
-      <c r="E71" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="M71">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="72" spans="5:13">
-      <c r="E72" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="M72">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" spans="5:13">
-      <c r="E73" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="M73">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="5:13">
-      <c r="E74" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="M74">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="5:13">
-      <c r="E75" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="M75">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="76" spans="5:13">
-      <c r="E76" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="M76">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="77" spans="5:13">
-      <c r="E77" s="5" t="s">
-        <v>105</v>
+      <c r="F77">
+        <v>25</v>
       </c>
       <c r="M77">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="78" spans="5:13">
-      <c r="E78" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="M78">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="5:13">
-      <c r="E79" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="M79">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="5:13">
-      <c r="E80" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="M80">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{6171A4A7-0979-4483-8022-2C371A704AAB}"/>
+    <hyperlink ref="C4:C27" r:id="rId2" display="ai1@kfq.com" xr:uid="{D6BCB0F2-78F2-4399-A4C6-234513669014}"/>
+    <hyperlink ref="C28" r:id="rId3" xr:uid="{241D7B22-3ED8-4B18-A658-FA21D11C4A22}"/>
+    <hyperlink ref="C29:C52" r:id="rId4" display="bigdata1@kfq.com" xr:uid="{3128DE31-EBA8-4BEC-8E0F-17140F5D6BDA}"/>
+    <hyperlink ref="C54:C77" r:id="rId5" display="smartfactory1@kfq.com" xr:uid="{04078668-B990-4137-BFB2-E4548C376F8E}"/>
+    <hyperlink ref="C53" r:id="rId6" xr:uid="{E8265AE3-105C-4A14-9929-45ED76F1EE3B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>